<commit_message>
rm useless images-source and update mos 838843cffb21c3a3c716e5d096d4625bb97329de
</commit_message>
<xml_diff>
--- a/nr-add-st/ig/ConceptMap-mos-cdl.xlsx
+++ b/nr-add-st/ig/ConceptMap-mos-cdl.xlsx
@@ -65,7 +65,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-07-22T10:07:53+00:00</t>
+    <t>2024-07-22T11:30:39+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -125,7 +125,7 @@
     <t>https://hl7.fr/ig/fhir/core/StructureDefinition/fr-core-related-person</t>
   </si>
   <si>
-    <t>PersonneTierce.idPersonneTierce</t>
+    <t>Contact.IdContact</t>
   </si>
   <si>
     <t>related-to</t>
@@ -134,13 +134,13 @@
     <t>RelatedPerson.identifier</t>
   </si>
   <si>
-    <t>PersonneTierce.adresse</t>
+    <t>Contact.adresse</t>
   </si>
   <si>
     <t>RelatedPerson.address</t>
   </si>
   <si>
-    <t>PersonneTierce.telecommunication</t>
+    <t>Contact.telecommunication</t>
   </si>
   <si>
     <t>RelatedPerson.telecom</t>

</xml_diff>